<commit_message>
Add v4 GGPPA analysis outputs and update variable summaries
</commit_message>
<xml_diff>
--- a/Analysis/v3 Output Excel/ggppa_progressivity_results_v3.xlsx
+++ b/Analysis/v3 Output Excel/ggppa_progressivity_results_v3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/zctpj17_ucl_ac_uk/Documents/ECON0053 Economics of Tax Policy/Grp Project/Quantitative/Analysis/v3 Output Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CA5E2659-48FF-B04A-A337-63EB1E806E29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{CA5E2659-48FF-B04A-A337-63EB1E806E29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E7D7C20-0E2E-5448-8763-CB3E5964D344}"/>
   <bookViews>
-    <workbookView xWindow="3980" yWindow="2780" windowWidth="28040" windowHeight="17180" xr2:uid="{BE33734D-A988-5044-A5D7-B714321DDBB4}"/>
+    <workbookView xWindow="0" yWindow="800" windowWidth="36000" windowHeight="21300" xr2:uid="{BE33734D-A988-5044-A5D7-B714321DDBB4}"/>
   </bookViews>
   <sheets>
     <sheet name="ggppa_progressivity_results_v3" sheetId="1" r:id="rId1"/>
@@ -315,7 +315,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -495,6 +495,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -656,9 +662,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -715,6 +722,57 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6F063318-E225-4140-9E13-F025C10F0B64}" name="Table1" displayName="Table1" ref="A1:AP141" totalsRowShown="0">
+  <autoFilter ref="A1:AP141" xr:uid="{6F063318-E225-4140-9E13-F025C10F0B64}"/>
+  <tableColumns count="42">
+    <tableColumn id="1" xr3:uid="{9757D10E-638B-A646-93F1-C89D00421545}" name="Province"/>
+    <tableColumn id="2" xr3:uid="{6FA370E3-7146-6C4E-B7BC-E17F96B961C9}" name="Year"/>
+    <tableColumn id="3" xr3:uid="{50ABB72F-F0D7-4740-98AC-C9457B77604F}" name="Quintile"/>
+    <tableColumn id="4" xr3:uid="{C82F832D-1698-6F4B-96B4-CBB8EABF177A}" name="Households"/>
+    <tableColumn id="5" xr3:uid="{BD75CB11-26AD-3945-86B8-A96F9708C8D6}" name="gas_exp"/>
+    <tableColumn id="6" xr3:uid="{69B43F91-50D5-7049-816F-5CCC4F710D1E}" name="ng_exp"/>
+    <tableColumn id="7" xr3:uid="{F8B77FA2-8CE1-B74D-87AF-007BF864ED9E}" name="oil_exp"/>
+    <tableColumn id="8" xr3:uid="{AF8B0984-A30C-2742-AF7D-72FDFE1CC362}" name="total_exp"/>
+    <tableColumn id="9" xr3:uid="{C371E37A-A7FE-AA44-8234-374476658729}" name="gasoline_price"/>
+    <tableColumn id="10" xr3:uid="{5A2967A3-F73E-E84A-846C-B13B31DAD283}" name="heating_oil_price"/>
+    <tableColumn id="11" xr3:uid="{70026B8F-C0C2-1E4F-A777-EBEE4F26191D}" name="Gasoline"/>
+    <tableColumn id="12" xr3:uid="{F4ED63EF-B6A6-8B4A-BB11-11B2AE90E9D1}" name="Light fuel oil"/>
+    <tableColumn id="13" xr3:uid="{8DE3E6D8-DDCF-9B45-84F9-5DD2B414FEF1}" name="Marketable natural gas"/>
+    <tableColumn id="14" xr3:uid="{772A6DC6-9057-B84B-8EA7-26555E5CED92}" name="ng_rate_per_GJ"/>
+    <tableColumn id="15" xr3:uid="{D5AA2C90-2255-794F-A721-BB61E0717527}" name="gasoline_litres"/>
+    <tableColumn id="16" xr3:uid="{544D2EA6-0273-9941-BCE1-F36FCF9BC3B8}" name="oil_litres"/>
+    <tableColumn id="17" xr3:uid="{3493EB8F-159E-1642-934F-28941C45FB9A}" name="ng_GJ"/>
+    <tableColumn id="18" xr3:uid="{72DFC50E-3D3B-3F4F-8773-2C3A50623BDE}" name="tax_gasoline"/>
+    <tableColumn id="19" xr3:uid="{D74EB328-F41A-1B44-948B-739B4542A8B3}" name="tax_oil"/>
+    <tableColumn id="20" xr3:uid="{5E566258-6A95-D64C-9788-2798332D6CCE}" name="tax_ng"/>
+    <tableColumn id="21" xr3:uid="{638DCF44-A7FB-2743-9E14-6E1923B21DAA}" name="direct_tax"/>
+    <tableColumn id="22" xr3:uid="{737B806F-94BA-804A-A7BA-10C05A1E4AD4}" name="gross_cost"/>
+    <tableColumn id="23" xr3:uid="{25A0564B-90D7-E748-9923-7ADAD42ED819}" name="CCR_single_base"/>
+    <tableColumn id="24" xr3:uid="{8734F946-B3AB-C542-A091-7F41A3E82F93}" name="CCR_couple_base"/>
+    <tableColumn id="25" xr3:uid="{C025788C-1AB9-9640-ABBC-0D716C9EC16A}" name="CCR_family4_base"/>
+    <tableColumn id="26" xr3:uid="{A375FB72-A3A2-6C4E-A3DB-32072872FCAC}" name="CCR_single_rural"/>
+    <tableColumn id="27" xr3:uid="{70990A7E-7867-B94D-9AF2-DF4BF75D3B35}" name="CCR_couple_rural"/>
+    <tableColumn id="28" xr3:uid="{2DBD0438-8C3A-B34B-B2D8-A26CE32D5821}" name="CCR_family4_rural"/>
+    <tableColumn id="29" xr3:uid="{518281BF-7359-DD4D-8885-4C1F67FB6ECC}" name="net_single_base"/>
+    <tableColumn id="30" xr3:uid="{448D0E50-DF41-EE42-9D6F-EBA88407CF24}" name="net_couple_base"/>
+    <tableColumn id="31" xr3:uid="{D85BE020-79C0-5D4E-83EA-7F1199E0F5ED}" name="net_family4_base"/>
+    <tableColumn id="32" xr3:uid="{D120DF0F-58EC-3B42-A1A4-B5969D809AA0}" name="net_single_rural"/>
+    <tableColumn id="33" xr3:uid="{9EF07715-ABE8-CB47-9CA3-A3453CEAE26B}" name="net_couple_rural"/>
+    <tableColumn id="34" xr3:uid="{C25DB80A-2026-7445-AAE0-0F6BFFD48310}" name="net_family4_rural"/>
+    <tableColumn id="35" xr3:uid="{F7FB52B9-2D6C-FF44-9E53-EE62A02A1054}" name="etr_direct_tax"/>
+    <tableColumn id="36" xr3:uid="{1083CB2F-D2BA-D245-A75C-19DE53018008}" name="etr_gross_cost"/>
+    <tableColumn id="37" xr3:uid="{2AD661E1-C670-B54D-84EE-B6DA04CEB9FA}" name="etr_net_single_base"/>
+    <tableColumn id="38" xr3:uid="{BFD10D22-2CF5-ED4A-809C-3F6969DA1DBD}" name="etr_net_couple_base"/>
+    <tableColumn id="39" xr3:uid="{A76FEE65-CF52-6046-917C-BA4018F2D2D0}" name="etr_net_family4_base"/>
+    <tableColumn id="40" xr3:uid="{6AF6A7C1-2393-C646-AECE-26DB32A62BA8}" name="etr_net_single_rural"/>
+    <tableColumn id="41" xr3:uid="{8D0937CB-CAC2-D04F-BE97-C92B7FF0A75A}" name="etr_net_couple_rural"/>
+    <tableColumn id="42" xr3:uid="{06C8696E-0D96-6142-804D-122EF4C253DD}" name="etr_net_family4_rural"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1036,11 +1094,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F82C009-CD8F-D747-8C56-7AFC7DE903BF}">
   <dimension ref="A1:AP141"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="W1" sqref="W1:X1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="42" width="10.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -1052,58 +1113,58 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
       <c r="V1" t="s">
@@ -18966,5 +19027,14 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{1faf88fe-a998-4c5b-93c9-210a11d9a5c2}" enabled="0" method="" siteId="{1faf88fe-a998-4c5b-93c9-210a11d9a5c2}" removed="1"/>
+</clbl:labelList>
 </file>
</xml_diff>